<commit_message>
Updates end Oct 21
</commit_message>
<xml_diff>
--- a/Inputs/IATI returns/Global Integrity - project data.xlsx
+++ b/Inputs/IATI returns/Global Integrity - project data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dfid-my.sharepoint.com/personal/e-clegg_dfid_gov_uk/Documents/PROJECT - MODARI/2. Awards/IATI/External partner data/2 - Completed returns/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/IATI returns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{5A7F9FE4-A58F-46C1-8A09-73E5DBA4578F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0F898E8E-15E2-4924-8F0E-D6E5BDB589BB}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{5A7F9FE4-A58F-46C1-8A09-73E5DBA4578F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{186D79DD-CA40-4E2A-9F44-EAEEC3CC6CFD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scope and Data Dictionary" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -203,9 +202,6 @@
     <t>Fund</t>
   </si>
   <si>
-    <t>FCDO fully funded</t>
-  </si>
-  <si>
     <t>Funder programme - IATI ID</t>
   </si>
   <si>
@@ -417,7 +413,10 @@
     <t>Uganda; Jamaica</t>
   </si>
   <si>
-    <t>FCDO partially funded</t>
+    <t>FCDO Research - Programmes</t>
+  </si>
+  <si>
+    <t>FCDO Research - Partnerships</t>
   </si>
 </sst>
 </file>
@@ -950,22 +949,22 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="119.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.58203125" customWidth="1"/>
-    <col min="5" max="5" width="24.75" customWidth="1"/>
-    <col min="6" max="25" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="39.296875" customWidth="1"/>
+    <col min="3" max="3" width="119.796875" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" customWidth="1"/>
+    <col min="5" max="5" width="24.69921875" customWidth="1"/>
+    <col min="6" max="25" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
@@ -973,34 +972,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>6</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>7</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>8</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>9</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>10</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>11</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>12</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>13</v>
       </c>
@@ -1154,7 +1153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>14</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>15</v>
       </c>
@@ -1174,995 +1173,995 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2179,32 +2178,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.796875" customWidth="1"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.796875" customWidth="1"/>
     <col min="4" max="4" width="26.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19.75" customWidth="1"/>
-    <col min="6" max="6" width="39.08203125" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="9" width="59.08203125" style="16" customWidth="1"/>
-    <col min="10" max="11" width="12.58203125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="17.75" style="29" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" customWidth="1"/>
+    <col min="6" max="6" width="39.09765625" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" customWidth="1"/>
+    <col min="8" max="9" width="59.09765625" style="16" customWidth="1"/>
+    <col min="10" max="11" width="12.59765625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="17.69921875" style="29" customWidth="1"/>
+    <col min="13" max="13" width="20.296875" customWidth="1"/>
     <col min="14" max="14" width="43" customWidth="1"/>
     <col min="15" max="15" width="25" customWidth="1"/>
-    <col min="16" max="16" width="29.08203125" customWidth="1"/>
+    <col min="16" max="16" width="29.09765625" customWidth="1"/>
     <col min="17" max="17" width="25" customWidth="1"/>
     <col min="18" max="18" width="46" customWidth="1"/>
-    <col min="19" max="21" width="8.58203125" customWidth="1"/>
+    <col min="19" max="21" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2215,10 +2212,10 @@
         <v>53</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>3</v>
@@ -2263,7 +2260,7 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2271,25 +2268,25 @@
         <v>52</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="J2" s="22">
         <v>43466</v>
@@ -2301,10 +2298,10 @@
         <v>318863</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O2" s="17" t="s">
         <v>48</v>
@@ -2313,7 +2310,7 @@
       <c r="Q2" s="12"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2321,25 +2318,25 @@
         <v>52</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G3" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J3" s="22">
         <v>43466</v>
@@ -2354,7 +2351,7 @@
         <v>50</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>49</v>
@@ -2363,7 +2360,7 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2371,25 +2368,25 @@
         <v>52</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="22">
         <v>43466</v>
@@ -2404,7 +2401,7 @@
         <v>44</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>46</v>
@@ -2413,7 +2410,7 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -2421,25 +2418,25 @@
         <v>52</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G5" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5" s="22">
         <v>43466</v>
@@ -2452,7 +2449,7 @@
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>48</v>
@@ -2461,7 +2458,7 @@
       <c r="Q5" s="12"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="6" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2469,25 +2466,25 @@
         <v>52</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G6" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="22">
         <v>43466</v>
@@ -2502,7 +2499,7 @@
         <v>45</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>48</v>
@@ -2511,7 +2508,7 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="14"/>
     </row>
-    <row r="7" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -2519,25 +2516,25 @@
         <v>52</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G7" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" s="22">
         <v>43466</v>
@@ -2550,7 +2547,7 @@
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>48</v>
@@ -2559,7 +2556,7 @@
       <c r="Q7" s="12"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2567,25 +2564,25 @@
         <v>52</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G8" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" s="22">
         <v>43466</v>
@@ -2600,7 +2597,7 @@
         <v>43</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>48</v>
@@ -2609,7 +2606,7 @@
       <c r="Q8" s="12"/>
       <c r="R8" s="14"/>
     </row>
-    <row r="9" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2617,25 +2614,25 @@
         <v>52</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G9" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J9" s="22">
         <v>43466</v>
@@ -2647,10 +2644,10 @@
         <v>347702</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O9" s="17" t="s">
         <v>48</v>
@@ -2659,7 +2656,7 @@
       <c r="Q9" s="12"/>
       <c r="R9" s="14"/>
     </row>
-    <row r="10" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2667,25 +2664,25 @@
         <v>52</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G10" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J10" s="22">
         <v>43466</v>
@@ -2697,23 +2694,23 @@
         <v>292564</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>48</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R10" s="14"/>
     </row>
-    <row r="11" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2721,25 +2718,25 @@
         <v>52</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G11" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J11" s="22">
         <v>43466</v>
@@ -2751,10 +2748,10 @@
         <v>349533</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O11" s="17" t="s">
         <v>46</v>
@@ -2763,7 +2760,7 @@
       <c r="Q11" s="12"/>
       <c r="R11" s="14"/>
     </row>
-    <row r="12" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -2771,25 +2768,25 @@
         <v>52</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G12" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J12" s="22">
         <v>43466</v>
@@ -2801,10 +2798,10 @@
         <v>349489</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O12" s="17" t="s">
         <v>48</v>
@@ -2813,7 +2810,7 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="14"/>
     </row>
-    <row r="13" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -2821,25 +2818,25 @@
         <v>52</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G13" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J13" s="22">
         <v>43466</v>
@@ -2851,10 +2848,10 @@
         <v>322686</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O13" s="17" t="s">
         <v>47</v>
@@ -2863,33 +2860,33 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G14" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J14" s="22">
         <v>43466</v>
@@ -2902,7 +2899,7 @@
       </c>
       <c r="M14" s="12"/>
       <c r="N14" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O14" s="17" t="s">
         <v>48</v>
@@ -2911,33 +2908,33 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="14"/>
     </row>
-    <row r="15" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G15" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="26">
         <v>43644</v>
@@ -2950,7 +2947,7 @@
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O15" s="17" t="s">
         <v>49</v>
@@ -2959,7 +2956,7 @@
       <c r="Q15" s="12"/>
       <c r="R15" s="14"/>
     </row>
-    <row r="16" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -2967,25 +2964,25 @@
         <v>52</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E16" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G16" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J16" s="22">
         <v>43739</v>
@@ -2997,10 +2994,10 @@
         <v>124135</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O16" s="17" t="s">
         <v>48</v>

</xml_diff>